<commit_message>
made changes in actions util
</commit_message>
<xml_diff>
--- a/testdata/Scenario1_CarWashContacts.xlsx
+++ b/testdata/Scenario1_CarWashContacts.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="163">
   <si>
     <t>Car Wash Name</t>
   </si>
@@ -453,6 +453,54 @@
   </si>
   <si>
     <t>07947137139</t>
+  </si>
+  <si>
+    <t>07947134354</t>
+  </si>
+  <si>
+    <t>07942682980</t>
+  </si>
+  <si>
+    <t>07947424969</t>
+  </si>
+  <si>
+    <t>07942688525</t>
+  </si>
+  <si>
+    <t>07947423715</t>
+  </si>
+  <si>
+    <t>07947147748</t>
+  </si>
+  <si>
+    <t>07947135961</t>
+  </si>
+  <si>
+    <t>07947129238</t>
+  </si>
+  <si>
+    <t>07947423933</t>
+  </si>
+  <si>
+    <t>07947104208</t>
+  </si>
+  <si>
+    <t>07947435989</t>
+  </si>
+  <si>
+    <t>07942694243</t>
+  </si>
+  <si>
+    <t>07942683662</t>
+  </si>
+  <si>
+    <t>07947152506</t>
+  </si>
+  <si>
+    <t>07947417537</t>
+  </si>
+  <si>
+    <t>07947110558</t>
   </si>
 </sst>
 </file>
@@ -516,7 +564,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s" s="0">
-        <v>142</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3">
@@ -524,7 +572,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s" s="0">
-        <v>143</v>
+        <v>160</v>
       </c>
     </row>
     <row r="4">
@@ -540,7 +588,7 @@
         <v>8</v>
       </c>
       <c r="B5" t="s" s="0">
-        <v>145</v>
+        <v>161</v>
       </c>
     </row>
     <row r="6">
@@ -548,7 +596,7 @@
         <v>10</v>
       </c>
       <c r="B6" t="s" s="0">
-        <v>146</v>
+        <v>162</v>
       </c>
     </row>
   </sheetData>

</xml_diff>